<commit_message>
Added VRF aware FHRP configuration feature in the code
</commit_message>
<xml_diff>
--- a/Cisco/ip_list_v0.xlsx
+++ b/Cisco/ip_list_v0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="switchnames" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="116">
   <si>
     <t xml:space="preserve">Host-names</t>
   </si>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">INBAND MGMT VRF</t>
   </si>
   <si>
+    <t xml:space="preserve">domain name</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample.sw01</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t xml:space="preserve">Management</t>
   </si>
   <si>
+    <t xml:space="preserve">test.local</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample.sw02</t>
   </si>
   <si>
@@ -161,124 +167,154 @@
     <t xml:space="preserve">gateway</t>
   </si>
   <si>
+    <t xml:space="preserve">Switch#1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priority1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch#2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priority2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.10.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.10.251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.10.252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vrrp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.20.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.20.254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.20.251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.10.20.252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interface ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vlan ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">portchannel ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLAG ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interface role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW Port IP address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subnet Mask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10G1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virtualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uplink_SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">portchannel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH1/49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">routed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.255.252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH1/50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH1/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.20.1.6</t>
+  </si>
+  <si>
     <t xml:space="preserve">switchname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.10.10.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.10.20.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.10.20.254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Host-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">switch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interface ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vlan ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purpose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portchannel ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLAG ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interface role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW Port IP address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subnet Mask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">server1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10G1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETH1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">virtualization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10G2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uplink_SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">portchannel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETH1/49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">routed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.20.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">255.255.255.252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETH1/50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.20.1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETH1/1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.20.1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.20.1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Loopback 10</t>
@@ -624,13 +660,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.69"/>
@@ -640,6 +676,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,258 +707,297 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -939,55 +1015,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.02"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,48 +1082,90 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1048,8 +1177,11 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1061,8 +1193,11 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1074,8 +1209,11 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1087,8 +1225,11 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1100,6 +1241,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1117,13 +1261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
@@ -1138,54 +1282,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>1</v>
@@ -1194,7 +1341,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>10</v>
@@ -1205,19 +1352,20 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>1</v>
@@ -1226,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>10</v>
@@ -1237,6 +1385,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
@@ -1251,6 +1400,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -1265,6 +1415,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -1279,6 +1430,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -1293,6 +1445,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
@@ -1307,6 +1460,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
@@ -1321,6 +1475,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
@@ -1335,6 +1490,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
@@ -1349,6 +1505,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
@@ -1363,6 +1520,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
@@ -1646,7 +1804,7 @@
       <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
@@ -1658,54 +1816,54 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
@@ -1718,27 +1876,27 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
@@ -1751,13 +1909,13 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,16 +1934,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>49</v>
@@ -1798,27 +1956,27 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>50</v>
@@ -1831,13 +1989,13 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1995,7 +2153,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.42"/>
@@ -2005,37 +2163,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3" t="str">
         <f aca="false">B2</f>
         <v>1.1.1.1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>10</v>
@@ -2044,17 +2202,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C3" s="3" t="str">
         <f aca="false">B3</f>
         <v>1.1.1.2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>10</v>
@@ -2063,17 +2221,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C4" s="3" t="str">
         <f aca="false">B4</f>
         <v>1.1.1.3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>10</v>
@@ -2082,17 +2240,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="str">
         <f aca="false">B5</f>
         <v>1.1.1.4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>10</v>
@@ -2101,17 +2259,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="str">
         <f aca="false">B6</f>
         <v>1.1.1.5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>10</v>
@@ -2120,17 +2278,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C7" s="3" t="str">
         <f aca="false">B7</f>
         <v>1.1.1.6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>10</v>
@@ -2139,17 +2297,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="str">
         <f aca="false">B8</f>
         <v>1.1.1.7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>10</v>
@@ -2158,17 +2316,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3" t="str">
         <f aca="false">B9</f>
         <v>1.1.1.8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>10</v>
@@ -2177,17 +2335,17 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="str">
         <f aca="false">B10</f>
         <v>1.1.1.9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>10</v>
@@ -2196,17 +2354,17 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C11" s="3" t="str">
         <f aca="false">B11</f>
         <v>1.1.1.10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>10</v>
@@ -2215,17 +2373,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C12" s="3" t="str">
         <f aca="false">B12</f>
         <v>1.1.1.11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>10</v>
@@ -2234,17 +2392,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C13" s="3" t="str">
         <f aca="false">B13</f>
         <v>1.1.1.12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>10</v>
@@ -2301,11 +2459,11 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.14"/>
@@ -2313,24 +2471,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1</v>
@@ -2341,7 +2499,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2</v>
@@ -2352,7 +2510,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>3</v>
@@ -2363,7 +2521,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
@@ -2374,7 +2532,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>2</v>
@@ -2385,7 +2543,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>3</v>
@@ -2396,7 +2554,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>5</v>
@@ -2407,7 +2565,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>6</v>
@@ -2418,7 +2576,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>7</v>
@@ -2429,7 +2587,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>5</v>
@@ -2440,7 +2598,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>6</v>
@@ -2451,7 +2609,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>7</v>
@@ -2462,7 +2620,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>8</v>
@@ -2473,7 +2631,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>9</v>
@@ -2484,7 +2642,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>10</v>
@@ -2495,7 +2653,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>8</v>
@@ -2506,7 +2664,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>9</v>
@@ -2517,7 +2675,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>10</v>
@@ -2528,7 +2686,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>11</v>
@@ -2539,7 +2697,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>12</v>
@@ -2550,7 +2708,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>13</v>
@@ -2561,7 +2719,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>11</v>
@@ -2572,7 +2730,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>12</v>
@@ -2583,7 +2741,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>13</v>
@@ -2594,7 +2752,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>14</v>
@@ -2605,7 +2763,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>15</v>
@@ -2616,7 +2774,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>16</v>
@@ -2627,7 +2785,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>14</v>
@@ -2638,7 +2796,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>15</v>
@@ -2649,7 +2807,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>16</v>
@@ -2660,7 +2818,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>17</v>
@@ -2668,7 +2826,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>18</v>
@@ -2676,7 +2834,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>19</v>
@@ -2684,7 +2842,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>17</v>
@@ -2692,7 +2850,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>18</v>
@@ -2700,7 +2858,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>19</v>
@@ -2708,7 +2866,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>20</v>
@@ -2716,7 +2874,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>21</v>
@@ -2724,7 +2882,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>22</v>
@@ -2732,7 +2890,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>20</v>
@@ -2740,7 +2898,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>21</v>
@@ -2748,7 +2906,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>22</v>
@@ -2756,7 +2914,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>23</v>
@@ -2764,7 +2922,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>24</v>
@@ -2772,7 +2930,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>25</v>
@@ -2780,7 +2938,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>23</v>
@@ -2788,7 +2946,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>24</v>
@@ -2796,7 +2954,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>25</v>
@@ -2804,7 +2962,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>26</v>
@@ -2812,7 +2970,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>27</v>
@@ -2820,7 +2978,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>28</v>
@@ -2828,7 +2986,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>26</v>
@@ -2836,7 +2994,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>27</v>
@@ -2844,7 +3002,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>28</v>
@@ -2852,7 +3010,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>29</v>
@@ -2860,7 +3018,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>30</v>
@@ -2868,7 +3026,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>31</v>
@@ -2876,7 +3034,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>29</v>
@@ -2884,7 +3042,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>30</v>
@@ -2892,7 +3050,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B62" s="2" t="n">
         <v>31</v>
@@ -2900,7 +3058,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B63" s="2" t="n">
         <v>32</v>
@@ -2908,7 +3066,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>32</v>
@@ -2916,7 +3074,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>33</v>
@@ -2924,7 +3082,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>33</v>

</xml_diff>